<commit_message>
[brown] 오타 수정  - initial plan import 수정
</commit_message>
<xml_diff>
--- a/baseball_schedule.xlsx
+++ b/baseball_schedule.xlsx
@@ -8,18 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonProjects\baseball_import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA55FFD-35DA-4031-993A-96BFD53D6A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AF58F7-AB4F-47EF-BEB5-282EA16E0B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{330C9D5B-CD97-489F-8826-7DF6997C54E6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{330C9D5B-CD97-489F-8826-7DF6997C54E6}"/>
   </bookViews>
   <sheets>
     <sheet name="matches" sheetId="5" r:id="rId1"/>
-    <sheet name="initial" sheetId="2" r:id="rId2"/>
-    <sheet name="teams" sheetId="3" r:id="rId3"/>
-    <sheet name="distanceMatrix" sheetId="4" r:id="rId4"/>
-    <sheet name="calendar" sheetId="1" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
+    <sheet name="initial" sheetId="2" r:id="rId3"/>
+    <sheet name="teams" sheetId="3" r:id="rId4"/>
+    <sheet name="distanceMatrix" sheetId="4" r:id="rId5"/>
+    <sheet name="calendar" sheetId="1" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">initial!$A$1:$D$277</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId7"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="61">
   <si>
     <t>datetime</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -227,6 +234,48 @@
     <t>consecutive</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>열 레이블</t>
+  </si>
+  <si>
+    <t>KIA</t>
+  </si>
+  <si>
+    <t>KT</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>SSG</t>
+  </si>
+  <si>
+    <t>두산</t>
+  </si>
+  <si>
+    <t>롯데</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>한화</t>
+  </si>
+  <si>
+    <t>총합계</t>
+  </si>
+  <si>
+    <t>행 레이블</t>
+  </si>
+  <si>
+    <t>합계 : consecutive</t>
+  </si>
 </sst>
 </file>
 
@@ -277,7 +326,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -285,6 +334,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -302,6 +360,1534 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="손혁준" refreshedDate="44591.462524768518" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="270" xr:uid="{BCC211F0-6064-4A74-88FB-C86BB99FCE45}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B1:D271" sheet="initial"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="AWAY" numFmtId="0">
+      <sharedItems count="10">
+        <s v="한화"/>
+        <s v="롯데"/>
+        <s v="삼성"/>
+        <s v="LG"/>
+        <s v="SSG"/>
+        <s v="NC"/>
+        <s v="KIA"/>
+        <s v="KT"/>
+        <s v="키움"/>
+        <s v="두산"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="HOME" numFmtId="0">
+      <sharedItems count="10">
+        <s v="두산"/>
+        <s v="키움"/>
+        <s v="KT"/>
+        <s v="KIA"/>
+        <s v="NC"/>
+        <s v="LG"/>
+        <s v="SSG"/>
+        <s v="한화"/>
+        <s v="삼성"/>
+        <s v="롯데"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="consecutive" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="3"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="270">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="7"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="5"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="9"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="7"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="9"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="5"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="8"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="9"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="7"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="5"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="7"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="9"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="4"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="5"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="8"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="4"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="7"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="8"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="6"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="6"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="7"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="9"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="5"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="8"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="9"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="4"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="6"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="7"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="8"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="9"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="7"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="9"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="5"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="8"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="9"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="6"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="8"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="6"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="6"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="8"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="4"/>
+    <n v="2"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5A093D1F-D290-438E-867A-70B4DEF230B6}" name="피벗 테이블1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:L15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisCol" showAll="0">
+      <items count="11">
+        <item x="6"/>
+        <item x="7"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="11">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="9"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="합계 : consecutive" fld="2" baseField="1" baseItem="3"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -601,10 +2187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E2ACCC-C017-4E9B-A090-E32B0D0F842D}">
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -771,7 +2357,7 @@
         <v>7</v>
       </c>
       <c r="C15">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
@@ -980,7 +2566,7 @@
         <v>11</v>
       </c>
       <c r="C34">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.4">
@@ -1112,7 +2698,7 @@
         <v>9</v>
       </c>
       <c r="C46">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.4">
@@ -1343,7 +2929,7 @@
         <v>13</v>
       </c>
       <c r="C67">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.4">
@@ -1420,7 +3006,7 @@
         <v>15</v>
       </c>
       <c r="C74">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.4">
@@ -1608,12 +3194,6 @@
       </c>
       <c r="C91">
         <v>8</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="C92">
-        <f>SUM(C2:C91)</f>
-        <v>720</v>
       </c>
     </row>
   </sheetData>
@@ -1623,11 +3203,480 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1DDD090-95DD-47B6-8700-44E738AC6B94}">
+  <dimension ref="A3:L15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="3.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.69921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5">
+        <v>8</v>
+      </c>
+      <c r="G5" s="5">
+        <v>8</v>
+      </c>
+      <c r="H5" s="5">
+        <v>8</v>
+      </c>
+      <c r="I5" s="5">
+        <v>8</v>
+      </c>
+      <c r="J5" s="5">
+        <v>8</v>
+      </c>
+      <c r="K5" s="5">
+        <v>8</v>
+      </c>
+      <c r="L5" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="5">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5">
+        <v>8</v>
+      </c>
+      <c r="G6" s="5">
+        <v>8</v>
+      </c>
+      <c r="H6" s="5">
+        <v>8</v>
+      </c>
+      <c r="I6" s="5">
+        <v>7</v>
+      </c>
+      <c r="J6" s="5">
+        <v>8</v>
+      </c>
+      <c r="K6" s="5">
+        <v>8</v>
+      </c>
+      <c r="L6" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="5">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5">
+        <v>8</v>
+      </c>
+      <c r="G7" s="5">
+        <v>8</v>
+      </c>
+      <c r="H7" s="5">
+        <v>8</v>
+      </c>
+      <c r="I7" s="5">
+        <v>8</v>
+      </c>
+      <c r="J7" s="5">
+        <v>8</v>
+      </c>
+      <c r="K7" s="5">
+        <v>8</v>
+      </c>
+      <c r="L7" s="5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="5">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5">
+        <v>7</v>
+      </c>
+      <c r="G8" s="5">
+        <v>8</v>
+      </c>
+      <c r="H8" s="5">
+        <v>8</v>
+      </c>
+      <c r="I8" s="5">
+        <v>8</v>
+      </c>
+      <c r="J8" s="5">
+        <v>8</v>
+      </c>
+      <c r="K8" s="5">
+        <v>8</v>
+      </c>
+      <c r="L8" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="5">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5">
+        <v>8</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5">
+        <v>8</v>
+      </c>
+      <c r="H9" s="5">
+        <v>8</v>
+      </c>
+      <c r="I9" s="5">
+        <v>8</v>
+      </c>
+      <c r="J9" s="5">
+        <v>8</v>
+      </c>
+      <c r="K9" s="5">
+        <v>8</v>
+      </c>
+      <c r="L9" s="5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="5">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5">
+        <v>8</v>
+      </c>
+      <c r="E10" s="5">
+        <v>8</v>
+      </c>
+      <c r="F10" s="5">
+        <v>8</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5">
+        <v>8</v>
+      </c>
+      <c r="I10" s="5">
+        <v>8</v>
+      </c>
+      <c r="J10" s="5">
+        <v>8</v>
+      </c>
+      <c r="K10" s="5">
+        <v>7</v>
+      </c>
+      <c r="L10" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="5">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5">
+        <v>8</v>
+      </c>
+      <c r="D11" s="5">
+        <v>8</v>
+      </c>
+      <c r="E11" s="5">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5">
+        <v>8</v>
+      </c>
+      <c r="G11" s="5">
+        <v>8</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5">
+        <v>8</v>
+      </c>
+      <c r="J11" s="5">
+        <v>8</v>
+      </c>
+      <c r="K11" s="5">
+        <v>8</v>
+      </c>
+      <c r="L11" s="5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="5">
+        <v>8</v>
+      </c>
+      <c r="C12" s="5">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5">
+        <v>8</v>
+      </c>
+      <c r="E12" s="5">
+        <v>8</v>
+      </c>
+      <c r="F12" s="5">
+        <v>8</v>
+      </c>
+      <c r="G12" s="5">
+        <v>8</v>
+      </c>
+      <c r="H12" s="5">
+        <v>8</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5">
+        <v>8</v>
+      </c>
+      <c r="K12" s="5">
+        <v>8</v>
+      </c>
+      <c r="L12" s="5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="5">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5">
+        <v>8</v>
+      </c>
+      <c r="D13" s="5">
+        <v>8</v>
+      </c>
+      <c r="E13" s="5">
+        <v>8</v>
+      </c>
+      <c r="F13" s="5">
+        <v>8</v>
+      </c>
+      <c r="G13" s="5">
+        <v>8</v>
+      </c>
+      <c r="H13" s="5">
+        <v>7</v>
+      </c>
+      <c r="I13" s="5">
+        <v>8</v>
+      </c>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5">
+        <v>8</v>
+      </c>
+      <c r="L13" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="5">
+        <v>8</v>
+      </c>
+      <c r="C14" s="5">
+        <v>8</v>
+      </c>
+      <c r="D14" s="5">
+        <v>8</v>
+      </c>
+      <c r="E14" s="5">
+        <v>8</v>
+      </c>
+      <c r="F14" s="5">
+        <v>8</v>
+      </c>
+      <c r="G14" s="5">
+        <v>8</v>
+      </c>
+      <c r="H14" s="5">
+        <v>8</v>
+      </c>
+      <c r="I14" s="5">
+        <v>8</v>
+      </c>
+      <c r="J14" s="5">
+        <v>8</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="5">
+        <v>72</v>
+      </c>
+      <c r="C15" s="5">
+        <v>72</v>
+      </c>
+      <c r="D15" s="5">
+        <v>71</v>
+      </c>
+      <c r="E15" s="5">
+        <v>72</v>
+      </c>
+      <c r="F15" s="5">
+        <v>71</v>
+      </c>
+      <c r="G15" s="5">
+        <v>72</v>
+      </c>
+      <c r="H15" s="5">
+        <v>71</v>
+      </c>
+      <c r="I15" s="5">
+        <v>71</v>
+      </c>
+      <c r="J15" s="5">
+        <v>72</v>
+      </c>
+      <c r="K15" s="5">
+        <v>71</v>
+      </c>
+      <c r="L15" s="5">
+        <v>715</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39CFE711-3122-4B1D-BBD3-577DDA921C51}">
   <dimension ref="A1:D277"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="A259" workbookViewId="0">
+      <selection activeCell="B273" sqref="B273:C277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4182,7 +6231,7 @@
         <v>6</v>
       </c>
       <c r="D182">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.4">
@@ -4196,7 +6245,7 @@
         <v>10</v>
       </c>
       <c r="D183">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.4">
@@ -4210,7 +6259,7 @@
         <v>7</v>
       </c>
       <c r="D184">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.4">
@@ -4224,7 +6273,7 @@
         <v>12</v>
       </c>
       <c r="D185">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.4">
@@ -4238,7 +6287,7 @@
         <v>14</v>
       </c>
       <c r="D186">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.4">
@@ -5429,6 +7478,12 @@
       </c>
       <c r="D271">
         <v>2</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D272">
+        <f>SUM(D1:D271)</f>
+        <v>715</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.4">
@@ -5481,13 +7536,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CD2A5A-A271-4674-9D08-E6494AEA3F25}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
@@ -5656,7 +7709,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28CE88E-77FD-49B9-A5FA-FFC7F298C90D}">
   <dimension ref="A1:E101"/>
   <sheetViews>
@@ -7593,11 +9646,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8672103-A1CA-4036-8B93-340C0DC8417A}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[brown] 오타 수정  - initial plan import 완료
</commit_message>
<xml_diff>
--- a/baseball_schedule.xlsx
+++ b/baseball_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonProjects\baseball_import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AF58F7-AB4F-47EF-BEB5-282EA16E0B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9082692-A4BB-43C7-96A5-1FAA6D79C73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{330C9D5B-CD97-489F-8826-7DF6997C54E6}"/>
   </bookViews>
@@ -21,7 +21,8 @@
     <sheet name="calendar" sheetId="1" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">initial!$A$1:$D$277</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">initial!$A$1:$D$271</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">matches!$A$1:$C$91</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -365,7 +366,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="손혁준" refreshedDate="44591.462524768518" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="270" xr:uid="{BCC211F0-6064-4A74-88FB-C86BB99FCE45}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="B1:D271" sheet="initial"/>
+    <worksheetSource ref="C1:D271" sheet="initial"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="AWAY" numFmtId="0">
@@ -3675,15 +3676,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39CFE711-3122-4B1D-BBD3-577DDA921C51}">
   <dimension ref="A1:D277"/>
   <sheetViews>
-    <sheetView topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="B273" sqref="B273:C277"/>
+    <sheetView topLeftCell="A251" workbookViewId="0">
+      <selection activeCell="C273" sqref="C273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
@@ -3691,10 +3692,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>46</v>
@@ -3705,10 +3706,10 @@
         <v>44288</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -3719,10 +3720,10 @@
         <v>44288</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -3733,10 +3734,10 @@
         <v>44288</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -3747,10 +3748,10 @@
         <v>44288</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -3761,10 +3762,10 @@
         <v>44288</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -3775,10 +3776,10 @@
         <v>44291</v>
       </c>
       <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -3789,10 +3790,10 @@
         <v>44291</v>
       </c>
       <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -3803,10 +3804,10 @@
         <v>44291</v>
       </c>
       <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>36</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -3817,10 +3818,10 @@
         <v>44291</v>
       </c>
       <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
         <v>37</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -3831,10 +3832,10 @@
         <v>44291</v>
       </c>
       <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -3845,10 +3846,10 @@
         <v>44294</v>
       </c>
       <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
         <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -3859,10 +3860,10 @@
         <v>44294</v>
       </c>
       <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
         <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -3873,10 +3874,10 @@
         <v>44294</v>
       </c>
       <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
         <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -3887,10 +3888,10 @@
         <v>44294</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -3901,10 +3902,10 @@
         <v>44294</v>
       </c>
       <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
         <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>9</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -3915,10 +3916,10 @@
         <v>44298</v>
       </c>
       <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
         <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -3929,10 +3930,10 @@
         <v>44298</v>
       </c>
       <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
         <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -3943,10 +3944,10 @@
         <v>44298</v>
       </c>
       <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
         <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -3957,10 +3958,10 @@
         <v>44298</v>
       </c>
       <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
         <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -3971,10 +3972,10 @@
         <v>44298</v>
       </c>
       <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
         <v>9</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -3985,10 +3986,10 @@
         <v>44301</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>3</v>
@@ -3999,10 +4000,10 @@
         <v>44301</v>
       </c>
       <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
         <v>11</v>
-      </c>
-      <c r="C23" t="s">
-        <v>15</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -4013,10 +4014,10 @@
         <v>44301</v>
       </c>
       <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
         <v>13</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -4027,10 +4028,10 @@
         <v>44301</v>
       </c>
       <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
         <v>10</v>
-      </c>
-      <c r="C25" t="s">
-        <v>9</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -4041,10 +4042,10 @@
         <v>44301</v>
       </c>
       <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
         <v>12</v>
-      </c>
-      <c r="C26" t="s">
-        <v>14</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -4055,10 +4056,10 @@
         <v>44305</v>
       </c>
       <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
         <v>10</v>
-      </c>
-      <c r="C27" t="s">
-        <v>13</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -4069,10 +4070,10 @@
         <v>44305</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D28">
         <v>3</v>
@@ -4083,10 +4084,10 @@
         <v>44305</v>
       </c>
       <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" t="s">
         <v>6</v>
-      </c>
-      <c r="C29" t="s">
-        <v>12</v>
       </c>
       <c r="D29">
         <v>3</v>
@@ -4097,10 +4098,10 @@
         <v>44305</v>
       </c>
       <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
         <v>7</v>
-      </c>
-      <c r="C30" t="s">
-        <v>9</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -4111,10 +4112,10 @@
         <v>44305</v>
       </c>
       <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
         <v>11</v>
-      </c>
-      <c r="C31" t="s">
-        <v>14</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -4125,10 +4126,10 @@
         <v>44308</v>
       </c>
       <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
         <v>13</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
       </c>
       <c r="D32">
         <v>3</v>
@@ -4139,10 +4140,10 @@
         <v>44308</v>
       </c>
       <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
         <v>12</v>
-      </c>
-      <c r="C33" t="s">
-        <v>8</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -4153,10 +4154,10 @@
         <v>44308</v>
       </c>
       <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
         <v>14</v>
-      </c>
-      <c r="C34" t="s">
-        <v>10</v>
       </c>
       <c r="D34">
         <v>3</v>
@@ -4167,10 +4168,10 @@
         <v>44308</v>
       </c>
       <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
         <v>15</v>
-      </c>
-      <c r="C35" t="s">
-        <v>7</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -4181,10 +4182,10 @@
         <v>44308</v>
       </c>
       <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
         <v>9</v>
-      </c>
-      <c r="C36" t="s">
-        <v>11</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -4195,10 +4196,10 @@
         <v>44312</v>
       </c>
       <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
         <v>14</v>
-      </c>
-      <c r="C37" t="s">
-        <v>6</v>
       </c>
       <c r="D37">
         <v>3</v>
@@ -4209,10 +4210,10 @@
         <v>44312</v>
       </c>
       <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
         <v>12</v>
-      </c>
-      <c r="C38" t="s">
-        <v>10</v>
       </c>
       <c r="D38">
         <v>3</v>
@@ -4223,10 +4224,10 @@
         <v>44312</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D39">
         <v>3</v>
@@ -4237,10 +4238,10 @@
         <v>44312</v>
       </c>
       <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
         <v>13</v>
-      </c>
-      <c r="C40" t="s">
-        <v>11</v>
       </c>
       <c r="D40">
         <v>3</v>
@@ -4251,10 +4252,10 @@
         <v>44312</v>
       </c>
       <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
         <v>15</v>
-      </c>
-      <c r="C41" t="s">
-        <v>9</v>
       </c>
       <c r="D41">
         <v>3</v>
@@ -4265,10 +4266,10 @@
         <v>44315</v>
       </c>
       <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" t="s">
         <v>9</v>
-      </c>
-      <c r="C42" t="s">
-        <v>13</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -4279,10 +4280,10 @@
         <v>44315</v>
       </c>
       <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
         <v>10</v>
-      </c>
-      <c r="C43" t="s">
-        <v>8</v>
       </c>
       <c r="D43">
         <v>3</v>
@@ -4293,10 +4294,10 @@
         <v>44315</v>
       </c>
       <c r="B44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" t="s">
         <v>6</v>
-      </c>
-      <c r="C44" t="s">
-        <v>15</v>
       </c>
       <c r="D44">
         <v>3</v>
@@ -4307,10 +4308,10 @@
         <v>44315</v>
       </c>
       <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" t="s">
         <v>11</v>
-      </c>
-      <c r="C45" t="s">
-        <v>12</v>
       </c>
       <c r="D45">
         <v>3</v>
@@ -4321,10 +4322,10 @@
         <v>44315</v>
       </c>
       <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" t="s">
         <v>7</v>
-      </c>
-      <c r="C46" t="s">
-        <v>14</v>
       </c>
       <c r="D46">
         <v>3</v>
@@ -4335,10 +4336,10 @@
         <v>44319</v>
       </c>
       <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" t="s">
         <v>6</v>
-      </c>
-      <c r="C47" t="s">
-        <v>13</v>
       </c>
       <c r="D47">
         <v>3</v>
@@ -4349,10 +4350,10 @@
         <v>44319</v>
       </c>
       <c r="B48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" t="s">
         <v>7</v>
-      </c>
-      <c r="C48" t="s">
-        <v>15</v>
       </c>
       <c r="D48">
         <v>3</v>
@@ -4363,10 +4364,10 @@
         <v>44319</v>
       </c>
       <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" t="s">
         <v>9</v>
-      </c>
-      <c r="C49" t="s">
-        <v>10</v>
       </c>
       <c r="D49">
         <v>3</v>
@@ -4377,10 +4378,10 @@
         <v>44319</v>
       </c>
       <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" t="s">
         <v>14</v>
-      </c>
-      <c r="C50" t="s">
-        <v>11</v>
       </c>
       <c r="D50">
         <v>3</v>
@@ -4391,10 +4392,10 @@
         <v>44319</v>
       </c>
       <c r="B51" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D51">
         <v>3</v>
@@ -4405,10 +4406,10 @@
         <v>44322</v>
       </c>
       <c r="B52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" t="s">
         <v>10</v>
-      </c>
-      <c r="C52" t="s">
-        <v>6</v>
       </c>
       <c r="D52">
         <v>3</v>
@@ -4419,10 +4420,10 @@
         <v>44322</v>
       </c>
       <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
         <v>15</v>
-      </c>
-      <c r="C53" t="s">
-        <v>8</v>
       </c>
       <c r="D53">
         <v>3</v>
@@ -4433,10 +4434,10 @@
         <v>44322</v>
       </c>
       <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
         <v>12</v>
-      </c>
-      <c r="C54" t="s">
-        <v>7</v>
       </c>
       <c r="D54">
         <v>3</v>
@@ -4447,10 +4448,10 @@
         <v>44322</v>
       </c>
       <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
         <v>11</v>
-      </c>
-      <c r="C55" t="s">
-        <v>9</v>
       </c>
       <c r="D55">
         <v>3</v>
@@ -4461,10 +4462,10 @@
         <v>44322</v>
       </c>
       <c r="B56" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" t="s">
         <v>13</v>
-      </c>
-      <c r="C56" t="s">
-        <v>14</v>
       </c>
       <c r="D56">
         <v>3</v>
@@ -4475,10 +4476,10 @@
         <v>44326</v>
       </c>
       <c r="B57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" t="s">
         <v>7</v>
-      </c>
-      <c r="C57" t="s">
-        <v>13</v>
       </c>
       <c r="D57">
         <v>3</v>
@@ -4489,10 +4490,10 @@
         <v>44326</v>
       </c>
       <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" t="s">
         <v>6</v>
-      </c>
-      <c r="C58" t="s">
-        <v>8</v>
       </c>
       <c r="D58">
         <v>3</v>
@@ -4503,10 +4504,10 @@
         <v>44326</v>
       </c>
       <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" t="s">
         <v>15</v>
-      </c>
-      <c r="C59" t="s">
-        <v>11</v>
       </c>
       <c r="D59">
         <v>3</v>
@@ -4517,10 +4518,10 @@
         <v>44326</v>
       </c>
       <c r="B60" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" t="s">
         <v>10</v>
-      </c>
-      <c r="C60" t="s">
-        <v>12</v>
       </c>
       <c r="D60">
         <v>3</v>
@@ -4531,10 +4532,10 @@
         <v>44326</v>
       </c>
       <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" t="s">
         <v>14</v>
-      </c>
-      <c r="C61" t="s">
-        <v>9</v>
       </c>
       <c r="D61">
         <v>3</v>
@@ -4545,10 +4546,10 @@
         <v>44329</v>
       </c>
       <c r="B62" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" t="s">
         <v>12</v>
-      </c>
-      <c r="C62" t="s">
-        <v>13</v>
       </c>
       <c r="D62">
         <v>3</v>
@@ -4559,10 +4560,10 @@
         <v>44329</v>
       </c>
       <c r="B63" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" t="s">
         <v>14</v>
-      </c>
-      <c r="C63" t="s">
-        <v>15</v>
       </c>
       <c r="D63">
         <v>3</v>
@@ -4573,10 +4574,10 @@
         <v>44329</v>
       </c>
       <c r="B64" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C64" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D64">
         <v>3</v>
@@ -4587,10 +4588,10 @@
         <v>44329</v>
       </c>
       <c r="B65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s">
         <v>9</v>
-      </c>
-      <c r="C65" t="s">
-        <v>7</v>
       </c>
       <c r="D65">
         <v>3</v>
@@ -4601,10 +4602,10 @@
         <v>44329</v>
       </c>
       <c r="B66" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" t="s">
         <v>6</v>
-      </c>
-      <c r="C66" t="s">
-        <v>11</v>
       </c>
       <c r="D66">
         <v>3</v>
@@ -4615,10 +4616,10 @@
         <v>44333</v>
       </c>
       <c r="B67" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" t="s">
         <v>15</v>
-      </c>
-      <c r="C67" t="s">
-        <v>6</v>
       </c>
       <c r="D67">
         <v>3</v>
@@ -4629,10 +4630,10 @@
         <v>44333</v>
       </c>
       <c r="B68" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" t="s">
         <v>13</v>
-      </c>
-      <c r="C68" t="s">
-        <v>10</v>
       </c>
       <c r="D68">
         <v>3</v>
@@ -4643,10 +4644,10 @@
         <v>44333</v>
       </c>
       <c r="B69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s">
         <v>11</v>
-      </c>
-      <c r="C69" t="s">
-        <v>7</v>
       </c>
       <c r="D69">
         <v>3</v>
@@ -4657,10 +4658,10 @@
         <v>44333</v>
       </c>
       <c r="B70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" t="s">
         <v>12</v>
-      </c>
-      <c r="C70" t="s">
-        <v>9</v>
       </c>
       <c r="D70">
         <v>3</v>
@@ -4671,10 +4672,10 @@
         <v>44333</v>
       </c>
       <c r="B71" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C71" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D71">
         <v>3</v>
@@ -4685,10 +4686,10 @@
         <v>44336</v>
       </c>
       <c r="B72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" t="s">
         <v>9</v>
-      </c>
-      <c r="C72" t="s">
-        <v>6</v>
       </c>
       <c r="D72">
         <v>3</v>
@@ -4699,10 +4700,10 @@
         <v>44336</v>
       </c>
       <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" t="s">
         <v>7</v>
-      </c>
-      <c r="C73" t="s">
-        <v>8</v>
       </c>
       <c r="D73">
         <v>3</v>
@@ -4713,10 +4714,10 @@
         <v>44336</v>
       </c>
       <c r="B74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" t="s">
         <v>13</v>
-      </c>
-      <c r="C74" t="s">
-        <v>15</v>
       </c>
       <c r="D74">
         <v>3</v>
@@ -4727,10 +4728,10 @@
         <v>44336</v>
       </c>
       <c r="B75" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75" t="s">
         <v>10</v>
-      </c>
-      <c r="C75" t="s">
-        <v>11</v>
       </c>
       <c r="D75">
         <v>3</v>
@@ -4741,10 +4742,10 @@
         <v>44336</v>
       </c>
       <c r="B76" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" t="s">
         <v>14</v>
-      </c>
-      <c r="C76" t="s">
-        <v>12</v>
       </c>
       <c r="D76">
         <v>3</v>
@@ -4755,10 +4756,10 @@
         <v>44340</v>
       </c>
       <c r="B77" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C77" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D77">
         <v>3</v>
@@ -4769,10 +4770,10 @@
         <v>44340</v>
       </c>
       <c r="B78" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" t="s">
         <v>9</v>
-      </c>
-      <c r="C78" t="s">
-        <v>15</v>
       </c>
       <c r="D78">
         <v>3</v>
@@ -4783,10 +4784,10 @@
         <v>44340</v>
       </c>
       <c r="B79" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s">
         <v>6</v>
-      </c>
-      <c r="C79" t="s">
-        <v>7</v>
       </c>
       <c r="D79">
         <v>3</v>
@@ -4797,10 +4798,10 @@
         <v>44340</v>
       </c>
       <c r="B80" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80" t="s">
         <v>12</v>
-      </c>
-      <c r="C80" t="s">
-        <v>11</v>
       </c>
       <c r="D80">
         <v>3</v>
@@ -4811,10 +4812,10 @@
         <v>44340</v>
       </c>
       <c r="B81" t="s">
+        <v>14</v>
+      </c>
+      <c r="C81" t="s">
         <v>10</v>
-      </c>
-      <c r="C81" t="s">
-        <v>14</v>
       </c>
       <c r="D81">
         <v>3</v>
@@ -4825,10 +4826,10 @@
         <v>44343</v>
       </c>
       <c r="B82" t="s">
+        <v>13</v>
+      </c>
+      <c r="C82" t="s">
         <v>11</v>
-      </c>
-      <c r="C82" t="s">
-        <v>13</v>
       </c>
       <c r="D82">
         <v>3</v>
@@ -4839,10 +4840,10 @@
         <v>44343</v>
       </c>
       <c r="B83" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" t="s">
         <v>7</v>
-      </c>
-      <c r="C83" t="s">
-        <v>10</v>
       </c>
       <c r="D83">
         <v>3</v>
@@ -4853,10 +4854,10 @@
         <v>44343</v>
       </c>
       <c r="B84" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" t="s">
         <v>15</v>
-      </c>
-      <c r="C84" t="s">
-        <v>12</v>
       </c>
       <c r="D84">
         <v>3</v>
@@ -4867,10 +4868,10 @@
         <v>44343</v>
       </c>
       <c r="B85" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C85" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D85">
         <v>3</v>
@@ -4881,10 +4882,10 @@
         <v>44343</v>
       </c>
       <c r="B86" t="s">
+        <v>14</v>
+      </c>
+      <c r="C86" t="s">
         <v>6</v>
-      </c>
-      <c r="C86" t="s">
-        <v>14</v>
       </c>
       <c r="D86">
         <v>3</v>
@@ -4895,10 +4896,10 @@
         <v>44347</v>
       </c>
       <c r="B87" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" t="s">
         <v>12</v>
-      </c>
-      <c r="C87" t="s">
-        <v>6</v>
       </c>
       <c r="D87">
         <v>3</v>
@@ -4909,10 +4910,10 @@
         <v>44347</v>
       </c>
       <c r="B88" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" t="s">
         <v>11</v>
-      </c>
-      <c r="C88" t="s">
-        <v>8</v>
       </c>
       <c r="D88">
         <v>3</v>
@@ -4923,10 +4924,10 @@
         <v>44347</v>
       </c>
       <c r="B89" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" t="s">
         <v>10</v>
-      </c>
-      <c r="C89" t="s">
-        <v>15</v>
       </c>
       <c r="D89">
         <v>3</v>
@@ -4937,10 +4938,10 @@
         <v>44347</v>
       </c>
       <c r="B90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" t="s">
         <v>14</v>
-      </c>
-      <c r="C90" t="s">
-        <v>7</v>
       </c>
       <c r="D90">
         <v>3</v>
@@ -4951,10 +4952,10 @@
         <v>44347</v>
       </c>
       <c r="B91" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" t="s">
         <v>13</v>
-      </c>
-      <c r="C91" t="s">
-        <v>9</v>
       </c>
       <c r="D91">
         <v>3</v>
@@ -4965,10 +4966,10 @@
         <v>44350</v>
       </c>
       <c r="B92" t="s">
+        <v>13</v>
+      </c>
+      <c r="C92" t="s">
         <v>15</v>
-      </c>
-      <c r="C92" t="s">
-        <v>13</v>
       </c>
       <c r="D92">
         <v>3</v>
@@ -4979,10 +4980,10 @@
         <v>44350</v>
       </c>
       <c r="B93" t="s">
+        <v>10</v>
+      </c>
+      <c r="C93" t="s">
         <v>12</v>
-      </c>
-      <c r="C93" t="s">
-        <v>10</v>
       </c>
       <c r="D93">
         <v>3</v>
@@ -4993,10 +4994,10 @@
         <v>44350</v>
       </c>
       <c r="B94" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C94" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D94">
         <v>3</v>
@@ -5007,10 +5008,10 @@
         <v>44350</v>
       </c>
       <c r="B95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C95" t="s">
         <v>6</v>
-      </c>
-      <c r="C95" t="s">
-        <v>11</v>
       </c>
       <c r="D95">
         <v>3</v>
@@ -5021,10 +5022,10 @@
         <v>44350</v>
       </c>
       <c r="B96" t="s">
+        <v>14</v>
+      </c>
+      <c r="C96" t="s">
         <v>9</v>
-      </c>
-      <c r="C96" t="s">
-        <v>14</v>
       </c>
       <c r="D96">
         <v>3</v>
@@ -5035,10 +5036,10 @@
         <v>44354</v>
       </c>
       <c r="B97" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97" t="s">
         <v>7</v>
-      </c>
-      <c r="C97" t="s">
-        <v>6</v>
       </c>
       <c r="D97">
         <v>3</v>
@@ -5049,10 +5050,10 @@
         <v>44354</v>
       </c>
       <c r="B98" t="s">
+        <v>8</v>
+      </c>
+      <c r="C98" t="s">
         <v>10</v>
-      </c>
-      <c r="C98" t="s">
-        <v>8</v>
       </c>
       <c r="D98">
         <v>3</v>
@@ -5063,10 +5064,10 @@
         <v>44354</v>
       </c>
       <c r="B99" t="s">
+        <v>12</v>
+      </c>
+      <c r="C99" t="s">
         <v>13</v>
-      </c>
-      <c r="C99" t="s">
-        <v>12</v>
       </c>
       <c r="D99">
         <v>3</v>
@@ -5077,10 +5078,10 @@
         <v>44354</v>
       </c>
       <c r="B100" t="s">
+        <v>9</v>
+      </c>
+      <c r="C100" t="s">
         <v>11</v>
-      </c>
-      <c r="C100" t="s">
-        <v>9</v>
       </c>
       <c r="D100">
         <v>3</v>
@@ -5091,10 +5092,10 @@
         <v>44354</v>
       </c>
       <c r="B101" t="s">
+        <v>14</v>
+      </c>
+      <c r="C101" t="s">
         <v>15</v>
-      </c>
-      <c r="C101" t="s">
-        <v>14</v>
       </c>
       <c r="D101">
         <v>3</v>
@@ -5105,10 +5106,10 @@
         <v>44357</v>
       </c>
       <c r="B102" t="s">
+        <v>13</v>
+      </c>
+      <c r="C102" t="s">
         <v>6</v>
-      </c>
-      <c r="C102" t="s">
-        <v>13</v>
       </c>
       <c r="D102">
         <v>3</v>
@@ -5119,10 +5120,10 @@
         <v>44357</v>
       </c>
       <c r="B103" t="s">
+        <v>15</v>
+      </c>
+      <c r="C103" t="s">
         <v>7</v>
-      </c>
-      <c r="C103" t="s">
-        <v>15</v>
       </c>
       <c r="D103">
         <v>3</v>
@@ -5133,10 +5134,10 @@
         <v>44357</v>
       </c>
       <c r="B104" t="s">
+        <v>11</v>
+      </c>
+      <c r="C104" t="s">
         <v>14</v>
-      </c>
-      <c r="C104" t="s">
-        <v>11</v>
       </c>
       <c r="D104">
         <v>3</v>
@@ -5147,10 +5148,10 @@
         <v>44357</v>
       </c>
       <c r="B105" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C105" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D105">
         <v>3</v>
@@ -5161,10 +5162,10 @@
         <v>44357</v>
       </c>
       <c r="B106" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106" t="s">
         <v>10</v>
-      </c>
-      <c r="C106" t="s">
-        <v>9</v>
       </c>
       <c r="D106">
         <v>3</v>
@@ -5175,10 +5176,10 @@
         <v>44361</v>
       </c>
       <c r="B107" t="s">
+        <v>13</v>
+      </c>
+      <c r="C107" t="s">
         <v>11</v>
-      </c>
-      <c r="C107" t="s">
-        <v>13</v>
       </c>
       <c r="D107">
         <v>3</v>
@@ -5189,10 +5190,10 @@
         <v>44361</v>
       </c>
       <c r="B108" t="s">
+        <v>8</v>
+      </c>
+      <c r="C108" t="s">
         <v>6</v>
-      </c>
-      <c r="C108" t="s">
-        <v>8</v>
       </c>
       <c r="D108">
         <v>3</v>
@@ -5203,10 +5204,10 @@
         <v>44361</v>
       </c>
       <c r="B109" t="s">
+        <v>10</v>
+      </c>
+      <c r="C109" t="s">
         <v>15</v>
-      </c>
-      <c r="C109" t="s">
-        <v>10</v>
       </c>
       <c r="D109">
         <v>3</v>
@@ -5217,10 +5218,10 @@
         <v>44361</v>
       </c>
       <c r="B110" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" t="s">
         <v>9</v>
-      </c>
-      <c r="C110" t="s">
-        <v>7</v>
       </c>
       <c r="D110">
         <v>3</v>
@@ -5231,10 +5232,10 @@
         <v>44361</v>
       </c>
       <c r="B111" t="s">
+        <v>14</v>
+      </c>
+      <c r="C111" t="s">
         <v>12</v>
-      </c>
-      <c r="C111" t="s">
-        <v>14</v>
       </c>
       <c r="D111">
         <v>3</v>
@@ -5245,10 +5246,10 @@
         <v>44364</v>
       </c>
       <c r="B112" t="s">
+        <v>6</v>
+      </c>
+      <c r="C112" t="s">
         <v>10</v>
-      </c>
-      <c r="C112" t="s">
-        <v>6</v>
       </c>
       <c r="D112">
         <v>3</v>
@@ -5259,10 +5260,10 @@
         <v>44364</v>
       </c>
       <c r="B113" t="s">
+        <v>8</v>
+      </c>
+      <c r="C113" t="s">
         <v>13</v>
-      </c>
-      <c r="C113" t="s">
-        <v>8</v>
       </c>
       <c r="D113">
         <v>3</v>
@@ -5273,10 +5274,10 @@
         <v>44364</v>
       </c>
       <c r="B114" t="s">
+        <v>12</v>
+      </c>
+      <c r="C114" t="s">
         <v>11</v>
-      </c>
-      <c r="C114" t="s">
-        <v>12</v>
       </c>
       <c r="D114">
         <v>3</v>
@@ -5287,10 +5288,10 @@
         <v>44364</v>
       </c>
       <c r="B115" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115" t="s">
         <v>15</v>
-      </c>
-      <c r="C115" t="s">
-        <v>9</v>
       </c>
       <c r="D115">
         <v>3</v>
@@ -5301,10 +5302,10 @@
         <v>44364</v>
       </c>
       <c r="B116" t="s">
+        <v>14</v>
+      </c>
+      <c r="C116" t="s">
         <v>7</v>
-      </c>
-      <c r="C116" t="s">
-        <v>14</v>
       </c>
       <c r="D116">
         <v>3</v>
@@ -5315,10 +5316,10 @@
         <v>44368</v>
       </c>
       <c r="B117" t="s">
+        <v>13</v>
+      </c>
+      <c r="C117" t="s">
         <v>7</v>
-      </c>
-      <c r="C117" t="s">
-        <v>13</v>
       </c>
       <c r="D117">
         <v>3</v>
@@ -5329,10 +5330,10 @@
         <v>44368</v>
       </c>
       <c r="B118" t="s">
+        <v>15</v>
+      </c>
+      <c r="C118" t="s">
         <v>6</v>
-      </c>
-      <c r="C118" t="s">
-        <v>15</v>
       </c>
       <c r="D118">
         <v>3</v>
@@ -5343,10 +5344,10 @@
         <v>44368</v>
       </c>
       <c r="B119" t="s">
+        <v>10</v>
+      </c>
+      <c r="C119" t="s">
         <v>14</v>
-      </c>
-      <c r="C119" t="s">
-        <v>10</v>
       </c>
       <c r="D119">
         <v>3</v>
@@ -5357,10 +5358,10 @@
         <v>44368</v>
       </c>
       <c r="B120" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C120" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D120">
         <v>3</v>
@@ -5371,10 +5372,10 @@
         <v>44368</v>
       </c>
       <c r="B121" t="s">
+        <v>12</v>
+      </c>
+      <c r="C121" t="s">
         <v>9</v>
-      </c>
-      <c r="C121" t="s">
-        <v>12</v>
       </c>
       <c r="D121">
         <v>3</v>
@@ -5385,10 +5386,10 @@
         <v>44371</v>
       </c>
       <c r="B122" t="s">
+        <v>6</v>
+      </c>
+      <c r="C122" t="s">
         <v>12</v>
-      </c>
-      <c r="C122" t="s">
-        <v>6</v>
       </c>
       <c r="D122">
         <v>3</v>
@@ -5399,10 +5400,10 @@
         <v>44371</v>
       </c>
       <c r="B123" t="s">
+        <v>15</v>
+      </c>
+      <c r="C123" t="s">
         <v>14</v>
-      </c>
-      <c r="C123" t="s">
-        <v>15</v>
       </c>
       <c r="D123">
         <v>3</v>
@@ -5413,10 +5414,10 @@
         <v>44371</v>
       </c>
       <c r="B124" t="s">
+        <v>10</v>
+      </c>
+      <c r="C124" t="s">
         <v>13</v>
-      </c>
-      <c r="C124" t="s">
-        <v>10</v>
       </c>
       <c r="D124">
         <v>3</v>
@@ -5427,10 +5428,10 @@
         <v>44371</v>
       </c>
       <c r="B125" t="s">
+        <v>7</v>
+      </c>
+      <c r="C125" t="s">
         <v>11</v>
-      </c>
-      <c r="C125" t="s">
-        <v>7</v>
       </c>
       <c r="D125">
         <v>3</v>
@@ -5441,10 +5442,10 @@
         <v>44371</v>
       </c>
       <c r="B126" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C126" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D126">
         <v>3</v>
@@ -5455,10 +5456,10 @@
         <v>44375</v>
       </c>
       <c r="B127" t="s">
+        <v>13</v>
+      </c>
+      <c r="C127" t="s">
         <v>14</v>
-      </c>
-      <c r="C127" t="s">
-        <v>13</v>
       </c>
       <c r="D127">
         <v>3</v>
@@ -5469,10 +5470,10 @@
         <v>44375</v>
       </c>
       <c r="B128" t="s">
+        <v>8</v>
+      </c>
+      <c r="C128" t="s">
         <v>12</v>
-      </c>
-      <c r="C128" t="s">
-        <v>8</v>
       </c>
       <c r="D128">
         <v>3</v>
@@ -5483,10 +5484,10 @@
         <v>44375</v>
       </c>
       <c r="B129" t="s">
+        <v>7</v>
+      </c>
+      <c r="C129" t="s">
         <v>15</v>
-      </c>
-      <c r="C129" t="s">
-        <v>7</v>
       </c>
       <c r="D129">
         <v>3</v>
@@ -5497,10 +5498,10 @@
         <v>44375</v>
       </c>
       <c r="B130" t="s">
+        <v>11</v>
+      </c>
+      <c r="C130" t="s">
         <v>10</v>
-      </c>
-      <c r="C130" t="s">
-        <v>11</v>
       </c>
       <c r="D130">
         <v>3</v>
@@ -5511,10 +5512,10 @@
         <v>44375</v>
       </c>
       <c r="B131" t="s">
+        <v>9</v>
+      </c>
+      <c r="C131" t="s">
         <v>6</v>
-      </c>
-      <c r="C131" t="s">
-        <v>9</v>
       </c>
       <c r="D131">
         <v>3</v>
@@ -5525,10 +5526,10 @@
         <v>44378</v>
       </c>
       <c r="B132" t="s">
+        <v>13</v>
+      </c>
+      <c r="C132" t="s">
         <v>9</v>
-      </c>
-      <c r="C132" t="s">
-        <v>13</v>
       </c>
       <c r="D132">
         <v>3</v>
@@ -5539,10 +5540,10 @@
         <v>44378</v>
       </c>
       <c r="B133" t="s">
+        <v>8</v>
+      </c>
+      <c r="C133" t="s">
         <v>7</v>
-      </c>
-      <c r="C133" t="s">
-        <v>8</v>
       </c>
       <c r="D133">
         <v>3</v>
@@ -5553,10 +5554,10 @@
         <v>44378</v>
       </c>
       <c r="B134" t="s">
+        <v>15</v>
+      </c>
+      <c r="C134" t="s">
         <v>12</v>
-      </c>
-      <c r="C134" t="s">
-        <v>15</v>
       </c>
       <c r="D134">
         <v>3</v>
@@ -5567,10 +5568,10 @@
         <v>44378</v>
       </c>
       <c r="B135" t="s">
+        <v>10</v>
+      </c>
+      <c r="C135" t="s">
         <v>6</v>
-      </c>
-      <c r="C135" t="s">
-        <v>10</v>
       </c>
       <c r="D135">
         <v>3</v>
@@ -5581,10 +5582,10 @@
         <v>44378</v>
       </c>
       <c r="B136" t="s">
+        <v>14</v>
+      </c>
+      <c r="C136" t="s">
         <v>11</v>
-      </c>
-      <c r="C136" t="s">
-        <v>14</v>
       </c>
       <c r="D136">
         <v>3</v>
@@ -5595,10 +5596,10 @@
         <v>44382</v>
       </c>
       <c r="B137" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C137" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D137">
         <v>3</v>
@@ -5609,10 +5610,10 @@
         <v>44382</v>
       </c>
       <c r="B138" t="s">
+        <v>15</v>
+      </c>
+      <c r="C138" t="s">
         <v>9</v>
-      </c>
-      <c r="C138" t="s">
-        <v>15</v>
       </c>
       <c r="D138">
         <v>3</v>
@@ -5623,10 +5624,10 @@
         <v>44382</v>
       </c>
       <c r="B139" t="s">
+        <v>7</v>
+      </c>
+      <c r="C139" t="s">
         <v>14</v>
-      </c>
-      <c r="C139" t="s">
-        <v>7</v>
       </c>
       <c r="D139">
         <v>3</v>
@@ -5637,10 +5638,10 @@
         <v>44382</v>
       </c>
       <c r="B140" t="s">
+        <v>11</v>
+      </c>
+      <c r="C140" t="s">
         <v>13</v>
-      </c>
-      <c r="C140" t="s">
-        <v>11</v>
       </c>
       <c r="D140">
         <v>3</v>
@@ -5651,10 +5652,10 @@
         <v>44382</v>
       </c>
       <c r="B141" t="s">
+        <v>12</v>
+      </c>
+      <c r="C141" t="s">
         <v>10</v>
-      </c>
-      <c r="C141" t="s">
-        <v>12</v>
       </c>
       <c r="D141">
         <v>3</v>
@@ -5665,10 +5666,10 @@
         <v>44385</v>
       </c>
       <c r="B142" t="s">
+        <v>6</v>
+      </c>
+      <c r="C142" t="s">
         <v>13</v>
-      </c>
-      <c r="C142" t="s">
-        <v>6</v>
       </c>
       <c r="D142">
         <v>3</v>
@@ -5679,10 +5680,10 @@
         <v>44385</v>
       </c>
       <c r="B143" t="s">
+        <v>8</v>
+      </c>
+      <c r="C143" t="s">
         <v>14</v>
-      </c>
-      <c r="C143" t="s">
-        <v>8</v>
       </c>
       <c r="D143">
         <v>3</v>
@@ -5693,10 +5694,10 @@
         <v>44385</v>
       </c>
       <c r="B144" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144" t="s">
         <v>9</v>
-      </c>
-      <c r="C144" t="s">
-        <v>10</v>
       </c>
       <c r="D144">
         <v>3</v>
@@ -5707,10 +5708,10 @@
         <v>44385</v>
       </c>
       <c r="B145" t="s">
+        <v>11</v>
+      </c>
+      <c r="C145" t="s">
         <v>15</v>
-      </c>
-      <c r="C145" t="s">
-        <v>11</v>
       </c>
       <c r="D145">
         <v>3</v>
@@ -5721,10 +5722,10 @@
         <v>44385</v>
       </c>
       <c r="B146" t="s">
+        <v>12</v>
+      </c>
+      <c r="C146" t="s">
         <v>7</v>
-      </c>
-      <c r="C146" t="s">
-        <v>12</v>
       </c>
       <c r="D146">
         <v>3</v>
@@ -5735,10 +5736,10 @@
         <v>44389</v>
       </c>
       <c r="B147" t="s">
+        <v>13</v>
+      </c>
+      <c r="C147" t="s">
         <v>12</v>
-      </c>
-      <c r="C147" t="s">
-        <v>13</v>
       </c>
       <c r="D147">
         <v>3</v>
@@ -5749,10 +5750,10 @@
         <v>44389</v>
       </c>
       <c r="B148" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C148" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D148">
         <v>3</v>
@@ -5763,10 +5764,10 @@
         <v>44389</v>
       </c>
       <c r="B149" t="s">
+        <v>10</v>
+      </c>
+      <c r="C149" t="s">
         <v>11</v>
-      </c>
-      <c r="C149" t="s">
-        <v>10</v>
       </c>
       <c r="D149">
         <v>3</v>
@@ -5777,10 +5778,10 @@
         <v>44389</v>
       </c>
       <c r="B150" t="s">
+        <v>9</v>
+      </c>
+      <c r="C150" t="s">
         <v>7</v>
-      </c>
-      <c r="C150" t="s">
-        <v>9</v>
       </c>
       <c r="D150">
         <v>3</v>
@@ -5791,10 +5792,10 @@
         <v>44389</v>
       </c>
       <c r="B151" t="s">
+        <v>14</v>
+      </c>
+      <c r="C151" t="s">
         <v>6</v>
-      </c>
-      <c r="C151" t="s">
-        <v>14</v>
       </c>
       <c r="D151">
         <v>3</v>
@@ -5805,10 +5806,10 @@
         <v>44399</v>
       </c>
       <c r="B152" t="s">
+        <v>6</v>
+      </c>
+      <c r="C152" t="s">
         <v>15</v>
-      </c>
-      <c r="C152" t="s">
-        <v>6</v>
       </c>
       <c r="D152">
         <v>3</v>
@@ -5819,10 +5820,10 @@
         <v>44399</v>
       </c>
       <c r="B153" t="s">
+        <v>8</v>
+      </c>
+      <c r="C153" t="s">
         <v>11</v>
-      </c>
-      <c r="C153" t="s">
-        <v>8</v>
       </c>
       <c r="D153">
         <v>3</v>
@@ -5833,10 +5834,10 @@
         <v>44399</v>
       </c>
       <c r="B154" t="s">
+        <v>7</v>
+      </c>
+      <c r="C154" t="s">
         <v>10</v>
-      </c>
-      <c r="C154" t="s">
-        <v>7</v>
       </c>
       <c r="D154">
         <v>3</v>
@@ -5847,10 +5848,10 @@
         <v>44399</v>
       </c>
       <c r="B155" t="s">
+        <v>9</v>
+      </c>
+      <c r="C155" t="s">
         <v>12</v>
-      </c>
-      <c r="C155" t="s">
-        <v>9</v>
       </c>
       <c r="D155">
         <v>3</v>
@@ -5861,10 +5862,10 @@
         <v>44399</v>
       </c>
       <c r="B156" t="s">
+        <v>14</v>
+      </c>
+      <c r="C156" t="s">
         <v>13</v>
-      </c>
-      <c r="C156" t="s">
-        <v>14</v>
       </c>
       <c r="D156">
         <v>3</v>
@@ -5875,10 +5876,10 @@
         <v>44403</v>
       </c>
       <c r="B157" t="s">
+        <v>6</v>
+      </c>
+      <c r="C157" t="s">
         <v>9</v>
-      </c>
-      <c r="C157" t="s">
-        <v>6</v>
       </c>
       <c r="D157">
         <v>3</v>
@@ -5889,10 +5890,10 @@
         <v>44403</v>
       </c>
       <c r="B158" t="s">
+        <v>15</v>
+      </c>
+      <c r="C158" t="s">
         <v>13</v>
-      </c>
-      <c r="C158" t="s">
-        <v>15</v>
       </c>
       <c r="D158">
         <v>3</v>
@@ -5903,10 +5904,10 @@
         <v>44403</v>
       </c>
       <c r="B159" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C159" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D159">
         <v>3</v>
@@ -5917,10 +5918,10 @@
         <v>44403</v>
       </c>
       <c r="B160" t="s">
+        <v>11</v>
+      </c>
+      <c r="C160" t="s">
         <v>7</v>
-      </c>
-      <c r="C160" t="s">
-        <v>11</v>
       </c>
       <c r="D160">
         <v>3</v>
@@ -5931,10 +5932,10 @@
         <v>44403</v>
       </c>
       <c r="B161" t="s">
+        <v>12</v>
+      </c>
+      <c r="C161" t="s">
         <v>14</v>
-      </c>
-      <c r="C161" t="s">
-        <v>12</v>
       </c>
       <c r="D161">
         <v>3</v>
@@ -5945,10 +5946,10 @@
         <v>44406</v>
       </c>
       <c r="B162" t="s">
+        <v>13</v>
+      </c>
+      <c r="C162" t="s">
         <v>10</v>
-      </c>
-      <c r="C162" t="s">
-        <v>13</v>
       </c>
       <c r="D162">
         <v>3</v>
@@ -5959,10 +5960,10 @@
         <v>44406</v>
       </c>
       <c r="B163" t="s">
+        <v>7</v>
+      </c>
+      <c r="C163" t="s">
         <v>6</v>
-      </c>
-      <c r="C163" t="s">
-        <v>7</v>
       </c>
       <c r="D163">
         <v>3</v>
@@ -5973,10 +5974,10 @@
         <v>44406</v>
       </c>
       <c r="B164" t="s">
+        <v>11</v>
+      </c>
+      <c r="C164" t="s">
         <v>9</v>
-      </c>
-      <c r="C164" t="s">
-        <v>11</v>
       </c>
       <c r="D164">
         <v>3</v>
@@ -5987,10 +5988,10 @@
         <v>44406</v>
       </c>
       <c r="B165" t="s">
+        <v>12</v>
+      </c>
+      <c r="C165" t="s">
         <v>15</v>
-      </c>
-      <c r="C165" t="s">
-        <v>12</v>
       </c>
       <c r="D165">
         <v>3</v>
@@ -6001,10 +6002,10 @@
         <v>44406</v>
       </c>
       <c r="B166" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C166" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D166">
         <v>3</v>
@@ -6015,10 +6016,10 @@
         <v>44410</v>
       </c>
       <c r="B167" t="s">
+        <v>6</v>
+      </c>
+      <c r="C167" t="s">
         <v>11</v>
-      </c>
-      <c r="C167" t="s">
-        <v>6</v>
       </c>
       <c r="D167">
         <v>3</v>
@@ -6029,10 +6030,10 @@
         <v>44410</v>
       </c>
       <c r="B168" t="s">
+        <v>8</v>
+      </c>
+      <c r="C168" t="s">
         <v>15</v>
-      </c>
-      <c r="C168" t="s">
-        <v>8</v>
       </c>
       <c r="D168">
         <v>3</v>
@@ -6043,10 +6044,10 @@
         <v>44410</v>
       </c>
       <c r="B169" t="s">
+        <v>7</v>
+      </c>
+      <c r="C169" t="s">
         <v>12</v>
-      </c>
-      <c r="C169" t="s">
-        <v>7</v>
       </c>
       <c r="D169">
         <v>3</v>
@@ -6057,10 +6058,10 @@
         <v>44410</v>
       </c>
       <c r="B170" t="s">
+        <v>9</v>
+      </c>
+      <c r="C170" t="s">
         <v>13</v>
-      </c>
-      <c r="C170" t="s">
-        <v>9</v>
       </c>
       <c r="D170">
         <v>3</v>
@@ -6071,10 +6072,10 @@
         <v>44410</v>
       </c>
       <c r="B171" t="s">
+        <v>14</v>
+      </c>
+      <c r="C171" t="s">
         <v>10</v>
-      </c>
-      <c r="C171" t="s">
-        <v>14</v>
       </c>
       <c r="D171">
         <v>3</v>
@@ -6085,10 +6086,10 @@
         <v>44413</v>
       </c>
       <c r="B172" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C172" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D172">
         <v>3</v>
@@ -6099,10 +6100,10 @@
         <v>44413</v>
       </c>
       <c r="B173" t="s">
+        <v>15</v>
+      </c>
+      <c r="C173" t="s">
         <v>11</v>
-      </c>
-      <c r="C173" t="s">
-        <v>15</v>
       </c>
       <c r="D173">
         <v>3</v>
@@ -6113,10 +6114,10 @@
         <v>44413</v>
       </c>
       <c r="B174" t="s">
+        <v>10</v>
+      </c>
+      <c r="C174" t="s">
         <v>7</v>
-      </c>
-      <c r="C174" t="s">
-        <v>10</v>
       </c>
       <c r="D174">
         <v>3</v>
@@ -6127,10 +6128,10 @@
         <v>44413</v>
       </c>
       <c r="B175" t="s">
+        <v>12</v>
+      </c>
+      <c r="C175" t="s">
         <v>6</v>
-      </c>
-      <c r="C175" t="s">
-        <v>12</v>
       </c>
       <c r="D175">
         <v>3</v>
@@ -6141,10 +6142,10 @@
         <v>44413</v>
       </c>
       <c r="B176" t="s">
+        <v>9</v>
+      </c>
+      <c r="C176" t="s">
         <v>14</v>
-      </c>
-      <c r="C176" t="s">
-        <v>9</v>
       </c>
       <c r="D176">
         <v>3</v>
@@ -6155,10 +6156,10 @@
         <v>44418</v>
       </c>
       <c r="B177" t="s">
+        <v>6</v>
+      </c>
+      <c r="C177" t="s">
         <v>14</v>
-      </c>
-      <c r="C177" t="s">
-        <v>6</v>
       </c>
       <c r="D177">
         <v>3</v>
@@ -6169,10 +6170,10 @@
         <v>44418</v>
       </c>
       <c r="B178" t="s">
+        <v>8</v>
+      </c>
+      <c r="C178" t="s">
         <v>9</v>
-      </c>
-      <c r="C178" t="s">
-        <v>8</v>
       </c>
       <c r="D178">
         <v>3</v>
@@ -6183,10 +6184,10 @@
         <v>44418</v>
       </c>
       <c r="B179" t="s">
+        <v>15</v>
+      </c>
+      <c r="C179" t="s">
         <v>10</v>
-      </c>
-      <c r="C179" t="s">
-        <v>15</v>
       </c>
       <c r="D179">
         <v>3</v>
@@ -6197,10 +6198,10 @@
         <v>44418</v>
       </c>
       <c r="B180" t="s">
+        <v>7</v>
+      </c>
+      <c r="C180" t="s">
         <v>13</v>
-      </c>
-      <c r="C180" t="s">
-        <v>7</v>
       </c>
       <c r="D180">
         <v>3</v>
@@ -6211,10 +6212,10 @@
         <v>44418</v>
       </c>
       <c r="B181" t="s">
+        <v>11</v>
+      </c>
+      <c r="C181" t="s">
         <v>12</v>
-      </c>
-      <c r="C181" t="s">
-        <v>11</v>
       </c>
       <c r="D181">
         <v>3</v>
@@ -6225,10 +6226,10 @@
         <v>44421</v>
       </c>
       <c r="B182" t="s">
+        <v>6</v>
+      </c>
+      <c r="C182" t="s">
         <v>15</v>
-      </c>
-      <c r="C182" t="s">
-        <v>6</v>
       </c>
       <c r="D182">
         <v>2</v>
@@ -6239,10 +6240,10 @@
         <v>44421</v>
       </c>
       <c r="B183" t="s">
+        <v>10</v>
+      </c>
+      <c r="C183" t="s">
         <v>11</v>
-      </c>
-      <c r="C183" t="s">
-        <v>10</v>
       </c>
       <c r="D183">
         <v>2</v>
@@ -6253,10 +6254,10 @@
         <v>44421</v>
       </c>
       <c r="B184" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C184" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D184">
         <v>2</v>
@@ -6267,10 +6268,10 @@
         <v>44421</v>
       </c>
       <c r="B185" t="s">
+        <v>12</v>
+      </c>
+      <c r="C185" t="s">
         <v>9</v>
-      </c>
-      <c r="C185" t="s">
-        <v>12</v>
       </c>
       <c r="D185">
         <v>2</v>
@@ -6281,10 +6282,10 @@
         <v>44421</v>
       </c>
       <c r="B186" t="s">
+        <v>14</v>
+      </c>
+      <c r="C186" t="s">
         <v>13</v>
-      </c>
-      <c r="C186" t="s">
-        <v>14</v>
       </c>
       <c r="D186">
         <v>2</v>
@@ -6295,10 +6296,10 @@
         <v>44424</v>
       </c>
       <c r="B187" t="s">
+        <v>13</v>
+      </c>
+      <c r="C187" t="s">
         <v>11</v>
-      </c>
-      <c r="C187" t="s">
-        <v>13</v>
       </c>
       <c r="D187">
         <v>2</v>
@@ -6309,10 +6310,10 @@
         <v>44424</v>
       </c>
       <c r="B188" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C188" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D188">
         <v>2</v>
@@ -6323,10 +6324,10 @@
         <v>44424</v>
       </c>
       <c r="B189" t="s">
+        <v>12</v>
+      </c>
+      <c r="C189" t="s">
         <v>15</v>
-      </c>
-      <c r="C189" t="s">
-        <v>12</v>
       </c>
       <c r="D189">
         <v>2</v>
@@ -6337,10 +6338,10 @@
         <v>44424</v>
       </c>
       <c r="B190" t="s">
+        <v>9</v>
+      </c>
+      <c r="C190" t="s">
         <v>6</v>
-      </c>
-      <c r="C190" t="s">
-        <v>9</v>
       </c>
       <c r="D190">
         <v>2</v>
@@ -6351,10 +6352,10 @@
         <v>44424</v>
       </c>
       <c r="B191" t="s">
+        <v>14</v>
+      </c>
+      <c r="C191" t="s">
         <v>7</v>
-      </c>
-      <c r="C191" t="s">
-        <v>14</v>
       </c>
       <c r="D191">
         <v>2</v>
@@ -6365,10 +6366,10 @@
         <v>44426</v>
       </c>
       <c r="B192" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C192" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D192">
         <v>2</v>
@@ -6379,10 +6380,10 @@
         <v>44426</v>
       </c>
       <c r="B193" t="s">
+        <v>15</v>
+      </c>
+      <c r="C193" t="s">
         <v>13</v>
-      </c>
-      <c r="C193" t="s">
-        <v>15</v>
       </c>
       <c r="D193">
         <v>2</v>
@@ -6393,10 +6394,10 @@
         <v>44426</v>
       </c>
       <c r="B194" t="s">
+        <v>7</v>
+      </c>
+      <c r="C194" t="s">
         <v>11</v>
-      </c>
-      <c r="C194" t="s">
-        <v>7</v>
       </c>
       <c r="D194">
         <v>2</v>
@@ -6407,10 +6408,10 @@
         <v>44426</v>
       </c>
       <c r="B195" t="s">
+        <v>12</v>
+      </c>
+      <c r="C195" t="s">
         <v>14</v>
-      </c>
-      <c r="C195" t="s">
-        <v>12</v>
       </c>
       <c r="D195">
         <v>2</v>
@@ -6421,10 +6422,10 @@
         <v>44426</v>
       </c>
       <c r="B196" t="s">
+        <v>9</v>
+      </c>
+      <c r="C196" t="s">
         <v>10</v>
-      </c>
-      <c r="C196" t="s">
-        <v>9</v>
       </c>
       <c r="D196">
         <v>2</v>
@@ -6435,10 +6436,10 @@
         <v>44428</v>
       </c>
       <c r="B197" t="s">
+        <v>13</v>
+      </c>
+      <c r="C197" t="s">
         <v>6</v>
-      </c>
-      <c r="C197" t="s">
-        <v>13</v>
       </c>
       <c r="D197">
         <v>2</v>
@@ -6449,10 +6450,10 @@
         <v>44428</v>
       </c>
       <c r="B198" t="s">
+        <v>8</v>
+      </c>
+      <c r="C198" t="s">
         <v>15</v>
-      </c>
-      <c r="C198" t="s">
-        <v>8</v>
       </c>
       <c r="D198">
         <v>2</v>
@@ -6463,10 +6464,10 @@
         <v>44428</v>
       </c>
       <c r="B199" t="s">
+        <v>10</v>
+      </c>
+      <c r="C199" t="s">
         <v>12</v>
-      </c>
-      <c r="C199" t="s">
-        <v>10</v>
       </c>
       <c r="D199">
         <v>2</v>
@@ -6477,10 +6478,10 @@
         <v>44428</v>
       </c>
       <c r="B200" t="s">
+        <v>11</v>
+      </c>
+      <c r="C200" t="s">
         <v>14</v>
-      </c>
-      <c r="C200" t="s">
-        <v>11</v>
       </c>
       <c r="D200">
         <v>2</v>
@@ -6491,10 +6492,10 @@
         <v>44428</v>
       </c>
       <c r="B201" t="s">
+        <v>9</v>
+      </c>
+      <c r="C201" t="s">
         <v>7</v>
-      </c>
-      <c r="C201" t="s">
-        <v>9</v>
       </c>
       <c r="D201">
         <v>2</v>
@@ -6505,10 +6506,10 @@
         <v>44431</v>
       </c>
       <c r="B202" t="s">
+        <v>6</v>
+      </c>
+      <c r="C202" t="s">
         <v>10</v>
-      </c>
-      <c r="C202" t="s">
-        <v>6</v>
       </c>
       <c r="D202">
         <v>2</v>
@@ -6519,10 +6520,10 @@
         <v>44431</v>
       </c>
       <c r="B203" t="s">
+        <v>8</v>
+      </c>
+      <c r="C203" t="s">
         <v>12</v>
-      </c>
-      <c r="C203" t="s">
-        <v>8</v>
       </c>
       <c r="D203">
         <v>2</v>
@@ -6533,10 +6534,10 @@
         <v>44431</v>
       </c>
       <c r="B204" t="s">
+        <v>15</v>
+      </c>
+      <c r="C204" t="s">
         <v>11</v>
-      </c>
-      <c r="C204" t="s">
-        <v>15</v>
       </c>
       <c r="D204">
         <v>2</v>
@@ -6547,10 +6548,10 @@
         <v>44431</v>
       </c>
       <c r="B205" t="s">
+        <v>7</v>
+      </c>
+      <c r="C205" t="s">
         <v>13</v>
-      </c>
-      <c r="C205" t="s">
-        <v>7</v>
       </c>
       <c r="D205">
         <v>2</v>
@@ -6561,10 +6562,10 @@
         <v>44431</v>
       </c>
       <c r="B206" t="s">
+        <v>14</v>
+      </c>
+      <c r="C206" t="s">
         <v>9</v>
-      </c>
-      <c r="C206" t="s">
-        <v>14</v>
       </c>
       <c r="D206">
         <v>2</v>
@@ -6575,10 +6576,10 @@
         <v>44433</v>
       </c>
       <c r="B207" t="s">
+        <v>13</v>
+      </c>
+      <c r="C207" t="s">
         <v>12</v>
-      </c>
-      <c r="C207" t="s">
-        <v>13</v>
       </c>
       <c r="D207">
         <v>2</v>
@@ -6589,10 +6590,10 @@
         <v>44433</v>
       </c>
       <c r="B208" t="s">
+        <v>10</v>
+      </c>
+      <c r="C208" t="s">
         <v>15</v>
-      </c>
-      <c r="C208" t="s">
-        <v>10</v>
       </c>
       <c r="D208">
         <v>2</v>
@@ -6603,10 +6604,10 @@
         <v>44433</v>
       </c>
       <c r="B209" t="s">
+        <v>7</v>
+      </c>
+      <c r="C209" t="s">
         <v>6</v>
-      </c>
-      <c r="C209" t="s">
-        <v>7</v>
       </c>
       <c r="D209">
         <v>2</v>
@@ -6617,10 +6618,10 @@
         <v>44433</v>
       </c>
       <c r="B210" t="s">
+        <v>9</v>
+      </c>
+      <c r="C210" t="s">
         <v>11</v>
-      </c>
-      <c r="C210" t="s">
-        <v>9</v>
       </c>
       <c r="D210">
         <v>2</v>
@@ -6631,10 +6632,10 @@
         <v>44433</v>
       </c>
       <c r="B211" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C211" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D211">
         <v>2</v>
@@ -6645,10 +6646,10 @@
         <v>44435</v>
       </c>
       <c r="B212" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C212" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D212">
         <v>2</v>
@@ -6659,10 +6660,10 @@
         <v>44435</v>
       </c>
       <c r="B213" t="s">
+        <v>15</v>
+      </c>
+      <c r="C213" t="s">
         <v>9</v>
-      </c>
-      <c r="C213" t="s">
-        <v>15</v>
       </c>
       <c r="D213">
         <v>2</v>
@@ -6673,10 +6674,10 @@
         <v>44435</v>
       </c>
       <c r="B214" t="s">
+        <v>11</v>
+      </c>
+      <c r="C214" t="s">
         <v>7</v>
-      </c>
-      <c r="C214" t="s">
-        <v>11</v>
       </c>
       <c r="D214">
         <v>2</v>
@@ -6687,10 +6688,10 @@
         <v>44435</v>
       </c>
       <c r="B215" t="s">
+        <v>12</v>
+      </c>
+      <c r="C215" t="s">
         <v>6</v>
-      </c>
-      <c r="C215" t="s">
-        <v>12</v>
       </c>
       <c r="D215">
         <v>2</v>
@@ -6701,10 +6702,10 @@
         <v>44435</v>
       </c>
       <c r="B216" t="s">
+        <v>14</v>
+      </c>
+      <c r="C216" t="s">
         <v>10</v>
-      </c>
-      <c r="C216" t="s">
-        <v>14</v>
       </c>
       <c r="D216">
         <v>2</v>
@@ -6715,10 +6716,10 @@
         <v>44438</v>
       </c>
       <c r="B217" t="s">
+        <v>13</v>
+      </c>
+      <c r="C217" t="s">
         <v>14</v>
-      </c>
-      <c r="C217" t="s">
-        <v>13</v>
       </c>
       <c r="D217">
         <v>2</v>
@@ -6729,10 +6730,10 @@
         <v>44438</v>
       </c>
       <c r="B218" t="s">
+        <v>8</v>
+      </c>
+      <c r="C218" t="s">
         <v>9</v>
-      </c>
-      <c r="C218" t="s">
-        <v>8</v>
       </c>
       <c r="D218">
         <v>2</v>
@@ -6743,10 +6744,10 @@
         <v>44438</v>
       </c>
       <c r="B219" t="s">
+        <v>10</v>
+      </c>
+      <c r="C219" t="s">
         <v>6</v>
-      </c>
-      <c r="C219" t="s">
-        <v>10</v>
       </c>
       <c r="D219">
         <v>2</v>
@@ -6757,10 +6758,10 @@
         <v>44438</v>
       </c>
       <c r="B220" t="s">
+        <v>7</v>
+      </c>
+      <c r="C220" t="s">
         <v>12</v>
-      </c>
-      <c r="C220" t="s">
-        <v>7</v>
       </c>
       <c r="D220">
         <v>2</v>
@@ -6771,10 +6772,10 @@
         <v>44438</v>
       </c>
       <c r="B221" t="s">
+        <v>11</v>
+      </c>
+      <c r="C221" t="s">
         <v>15</v>
-      </c>
-      <c r="C221" t="s">
-        <v>11</v>
       </c>
       <c r="D221">
         <v>2</v>
@@ -6785,10 +6786,10 @@
         <v>44440</v>
       </c>
       <c r="B222" t="s">
+        <v>6</v>
+      </c>
+      <c r="C222" t="s">
         <v>9</v>
-      </c>
-      <c r="C222" t="s">
-        <v>6</v>
       </c>
       <c r="D222">
         <v>2</v>
@@ -6799,10 +6800,10 @@
         <v>44440</v>
       </c>
       <c r="B223" t="s">
+        <v>8</v>
+      </c>
+      <c r="C223" t="s">
         <v>7</v>
-      </c>
-      <c r="C223" t="s">
-        <v>8</v>
       </c>
       <c r="D223">
         <v>2</v>
@@ -6813,10 +6814,10 @@
         <v>44440</v>
       </c>
       <c r="B224" t="s">
+        <v>15</v>
+      </c>
+      <c r="C224" t="s">
         <v>14</v>
-      </c>
-      <c r="C224" t="s">
-        <v>15</v>
       </c>
       <c r="D224">
         <v>2</v>
@@ -6827,10 +6828,10 @@
         <v>44440</v>
       </c>
       <c r="B225" t="s">
+        <v>10</v>
+      </c>
+      <c r="C225" t="s">
         <v>13</v>
-      </c>
-      <c r="C225" t="s">
-        <v>10</v>
       </c>
       <c r="D225">
         <v>2</v>
@@ -6841,10 +6842,10 @@
         <v>44440</v>
       </c>
       <c r="B226" t="s">
+        <v>12</v>
+      </c>
+      <c r="C226" t="s">
         <v>11</v>
-      </c>
-      <c r="C226" t="s">
-        <v>12</v>
       </c>
       <c r="D226">
         <v>2</v>
@@ -6855,10 +6856,10 @@
         <v>44442</v>
       </c>
       <c r="B227" t="s">
+        <v>6</v>
+      </c>
+      <c r="C227" t="s">
         <v>11</v>
-      </c>
-      <c r="C227" t="s">
-        <v>6</v>
       </c>
       <c r="D227">
         <v>2</v>
@@ -6869,10 +6870,10 @@
         <v>44442</v>
       </c>
       <c r="B228" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C228" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D228">
         <v>2</v>
@@ -6883,10 +6884,10 @@
         <v>44442</v>
       </c>
       <c r="B229" t="s">
+        <v>7</v>
+      </c>
+      <c r="C229" t="s">
         <v>14</v>
-      </c>
-      <c r="C229" t="s">
-        <v>7</v>
       </c>
       <c r="D229">
         <v>2</v>
@@ -6897,10 +6898,10 @@
         <v>44442</v>
       </c>
       <c r="B230" t="s">
+        <v>12</v>
+      </c>
+      <c r="C230" t="s">
         <v>10</v>
-      </c>
-      <c r="C230" t="s">
-        <v>12</v>
       </c>
       <c r="D230">
         <v>2</v>
@@ -6911,10 +6912,10 @@
         <v>44442</v>
       </c>
       <c r="B231" t="s">
+        <v>9</v>
+      </c>
+      <c r="C231" t="s">
         <v>13</v>
-      </c>
-      <c r="C231" t="s">
-        <v>9</v>
       </c>
       <c r="D231">
         <v>2</v>
@@ -6925,10 +6926,10 @@
         <v>44445</v>
       </c>
       <c r="B232" t="s">
+        <v>13</v>
+      </c>
+      <c r="C232" t="s">
         <v>15</v>
-      </c>
-      <c r="C232" t="s">
-        <v>13</v>
       </c>
       <c r="D232">
         <v>2</v>
@@ -6939,10 +6940,10 @@
         <v>44445</v>
       </c>
       <c r="B233" t="s">
+        <v>10</v>
+      </c>
+      <c r="C233" t="s">
         <v>7</v>
-      </c>
-      <c r="C233" t="s">
-        <v>10</v>
       </c>
       <c r="D233">
         <v>2</v>
@@ -6953,10 +6954,10 @@
         <v>44445</v>
       </c>
       <c r="B234" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C234" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D234">
         <v>2</v>
@@ -6967,10 +6968,10 @@
         <v>44445</v>
       </c>
       <c r="B235" t="s">
+        <v>9</v>
+      </c>
+      <c r="C235" t="s">
         <v>12</v>
-      </c>
-      <c r="C235" t="s">
-        <v>9</v>
       </c>
       <c r="D235">
         <v>2</v>
@@ -6981,10 +6982,10 @@
         <v>44445</v>
       </c>
       <c r="B236" t="s">
+        <v>14</v>
+      </c>
+      <c r="C236" t="s">
         <v>6</v>
-      </c>
-      <c r="C236" t="s">
-        <v>14</v>
       </c>
       <c r="D236">
         <v>2</v>
@@ -6995,10 +6996,10 @@
         <v>44447</v>
       </c>
       <c r="B237" t="s">
+        <v>6</v>
+      </c>
+      <c r="C237" t="s">
         <v>7</v>
-      </c>
-      <c r="C237" t="s">
-        <v>6</v>
       </c>
       <c r="D237">
         <v>2</v>
@@ -7009,10 +7010,10 @@
         <v>44447</v>
       </c>
       <c r="B238" t="s">
+        <v>8</v>
+      </c>
+      <c r="C238" t="s">
         <v>13</v>
-      </c>
-      <c r="C238" t="s">
-        <v>8</v>
       </c>
       <c r="D238">
         <v>2</v>
@@ -7023,10 +7024,10 @@
         <v>44447</v>
       </c>
       <c r="B239" t="s">
+        <v>15</v>
+      </c>
+      <c r="C239" t="s">
         <v>12</v>
-      </c>
-      <c r="C239" t="s">
-        <v>15</v>
       </c>
       <c r="D239">
         <v>2</v>
@@ -7037,10 +7038,10 @@
         <v>44447</v>
       </c>
       <c r="B240" t="s">
+        <v>10</v>
+      </c>
+      <c r="C240" t="s">
         <v>14</v>
-      </c>
-      <c r="C240" t="s">
-        <v>10</v>
       </c>
       <c r="D240">
         <v>2</v>
@@ -7051,10 +7052,10 @@
         <v>44447</v>
       </c>
       <c r="B241" t="s">
+        <v>11</v>
+      </c>
+      <c r="C241" t="s">
         <v>9</v>
-      </c>
-      <c r="C241" t="s">
-        <v>11</v>
       </c>
       <c r="D241">
         <v>2</v>
@@ -7065,10 +7066,10 @@
         <v>44449</v>
       </c>
       <c r="B242" t="s">
+        <v>6</v>
+      </c>
+      <c r="C242" t="s">
         <v>12</v>
-      </c>
-      <c r="C242" t="s">
-        <v>6</v>
       </c>
       <c r="D242">
         <v>2</v>
@@ -7079,10 +7080,10 @@
         <v>44449</v>
       </c>
       <c r="B243" t="s">
+        <v>8</v>
+      </c>
+      <c r="C243" t="s">
         <v>10</v>
-      </c>
-      <c r="C243" t="s">
-        <v>8</v>
       </c>
       <c r="D243">
         <v>2</v>
@@ -7093,10 +7094,10 @@
         <v>44449</v>
       </c>
       <c r="B244" t="s">
+        <v>7</v>
+      </c>
+      <c r="C244" t="s">
         <v>15</v>
-      </c>
-      <c r="C244" t="s">
-        <v>7</v>
       </c>
       <c r="D244">
         <v>2</v>
@@ -7107,10 +7108,10 @@
         <v>44449</v>
       </c>
       <c r="B245" t="s">
+        <v>11</v>
+      </c>
+      <c r="C245" t="s">
         <v>13</v>
-      </c>
-      <c r="C245" t="s">
-        <v>11</v>
       </c>
       <c r="D245">
         <v>2</v>
@@ -7121,10 +7122,10 @@
         <v>44449</v>
       </c>
       <c r="B246" t="s">
+        <v>9</v>
+      </c>
+      <c r="C246" t="s">
         <v>14</v>
-      </c>
-      <c r="C246" t="s">
-        <v>9</v>
       </c>
       <c r="D246">
         <v>2</v>
@@ -7135,10 +7136,10 @@
         <v>44452</v>
       </c>
       <c r="B247" t="s">
+        <v>6</v>
+      </c>
+      <c r="C247" t="s">
         <v>13</v>
-      </c>
-      <c r="C247" t="s">
-        <v>6</v>
       </c>
       <c r="D247">
         <v>2</v>
@@ -7149,10 +7150,10 @@
         <v>44452</v>
       </c>
       <c r="B248" t="s">
+        <v>7</v>
+      </c>
+      <c r="C248" t="s">
         <v>10</v>
-      </c>
-      <c r="C248" t="s">
-        <v>7</v>
       </c>
       <c r="D248">
         <v>2</v>
@@ -7163,10 +7164,10 @@
         <v>44452</v>
       </c>
       <c r="B249" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C249" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D249">
         <v>2</v>
@@ -7177,10 +7178,10 @@
         <v>44452</v>
       </c>
       <c r="B250" t="s">
+        <v>9</v>
+      </c>
+      <c r="C250" t="s">
         <v>15</v>
-      </c>
-      <c r="C250" t="s">
-        <v>9</v>
       </c>
       <c r="D250">
         <v>2</v>
@@ -7191,10 +7192,10 @@
         <v>44452</v>
       </c>
       <c r="B251" t="s">
+        <v>14</v>
+      </c>
+      <c r="C251" t="s">
         <v>11</v>
-      </c>
-      <c r="C251" t="s">
-        <v>14</v>
       </c>
       <c r="D251">
         <v>2</v>
@@ -7205,10 +7206,10 @@
         <v>44454</v>
       </c>
       <c r="B252" t="s">
+        <v>13</v>
+      </c>
+      <c r="C252" t="s">
         <v>10</v>
-      </c>
-      <c r="C252" t="s">
-        <v>13</v>
       </c>
       <c r="D252">
         <v>2</v>
@@ -7219,10 +7220,10 @@
         <v>44454</v>
       </c>
       <c r="B253" t="s">
+        <v>11</v>
+      </c>
+      <c r="C253" t="s">
         <v>6</v>
-      </c>
-      <c r="C253" t="s">
-        <v>11</v>
       </c>
       <c r="D253">
         <v>2</v>
@@ -7233,10 +7234,10 @@
         <v>44454</v>
       </c>
       <c r="B254" t="s">
+        <v>12</v>
+      </c>
+      <c r="C254" t="s">
         <v>7</v>
-      </c>
-      <c r="C254" t="s">
-        <v>12</v>
       </c>
       <c r="D254">
         <v>2</v>
@@ -7247,10 +7248,10 @@
         <v>44454</v>
       </c>
       <c r="B255" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C255" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D255">
         <v>2</v>
@@ -7261,10 +7262,10 @@
         <v>44454</v>
       </c>
       <c r="B256" t="s">
+        <v>14</v>
+      </c>
+      <c r="C256" t="s">
         <v>15</v>
-      </c>
-      <c r="C256" t="s">
-        <v>14</v>
       </c>
       <c r="D256">
         <v>2</v>
@@ -7275,10 +7276,10 @@
         <v>44456</v>
       </c>
       <c r="B257" t="s">
+        <v>13</v>
+      </c>
+      <c r="C257" t="s">
         <v>7</v>
-      </c>
-      <c r="C257" t="s">
-        <v>13</v>
       </c>
       <c r="D257">
         <v>2</v>
@@ -7289,10 +7290,10 @@
         <v>44456</v>
       </c>
       <c r="B258" t="s">
+        <v>8</v>
+      </c>
+      <c r="C258" t="s">
         <v>14</v>
-      </c>
-      <c r="C258" t="s">
-        <v>8</v>
       </c>
       <c r="D258">
         <v>2</v>
@@ -7303,10 +7304,10 @@
         <v>44456</v>
       </c>
       <c r="B259" t="s">
+        <v>15</v>
+      </c>
+      <c r="C259" t="s">
         <v>6</v>
-      </c>
-      <c r="C259" t="s">
-        <v>15</v>
       </c>
       <c r="D259">
         <v>2</v>
@@ -7317,10 +7318,10 @@
         <v>44456</v>
       </c>
       <c r="B260" t="s">
+        <v>10</v>
+      </c>
+      <c r="C260" t="s">
         <v>9</v>
-      </c>
-      <c r="C260" t="s">
-        <v>10</v>
       </c>
       <c r="D260">
         <v>2</v>
@@ -7331,10 +7332,10 @@
         <v>44456</v>
       </c>
       <c r="B261" t="s">
+        <v>11</v>
+      </c>
+      <c r="C261" t="s">
         <v>12</v>
-      </c>
-      <c r="C261" t="s">
-        <v>11</v>
       </c>
       <c r="D261">
         <v>2</v>
@@ -7345,10 +7346,10 @@
         <v>44459</v>
       </c>
       <c r="B262" t="s">
+        <v>6</v>
+      </c>
+      <c r="C262" t="s">
         <v>14</v>
-      </c>
-      <c r="C262" t="s">
-        <v>6</v>
       </c>
       <c r="D262">
         <v>2</v>
@@ -7359,10 +7360,10 @@
         <v>44459</v>
       </c>
       <c r="B263" t="s">
+        <v>8</v>
+      </c>
+      <c r="C263" t="s">
         <v>11</v>
-      </c>
-      <c r="C263" t="s">
-        <v>8</v>
       </c>
       <c r="D263">
         <v>2</v>
@@ -7373,10 +7374,10 @@
         <v>44459</v>
       </c>
       <c r="B264" t="s">
+        <v>15</v>
+      </c>
+      <c r="C264" t="s">
         <v>10</v>
-      </c>
-      <c r="C264" t="s">
-        <v>15</v>
       </c>
       <c r="D264">
         <v>2</v>
@@ -7387,10 +7388,10 @@
         <v>44459</v>
       </c>
       <c r="B265" t="s">
+        <v>7</v>
+      </c>
+      <c r="C265" t="s">
         <v>9</v>
-      </c>
-      <c r="C265" t="s">
-        <v>7</v>
       </c>
       <c r="D265">
         <v>2</v>
@@ -7401,10 +7402,10 @@
         <v>44459</v>
       </c>
       <c r="B266" t="s">
+        <v>12</v>
+      </c>
+      <c r="C266" t="s">
         <v>13</v>
-      </c>
-      <c r="C266" t="s">
-        <v>12</v>
       </c>
       <c r="D266">
         <v>2</v>
@@ -7415,10 +7416,10 @@
         <v>44461</v>
       </c>
       <c r="B267" t="s">
+        <v>13</v>
+      </c>
+      <c r="C267" t="s">
         <v>9</v>
-      </c>
-      <c r="C267" t="s">
-        <v>13</v>
       </c>
       <c r="D267">
         <v>2</v>
@@ -7429,10 +7430,10 @@
         <v>44461</v>
       </c>
       <c r="B268" t="s">
+        <v>8</v>
+      </c>
+      <c r="C268" t="s">
         <v>6</v>
-      </c>
-      <c r="C268" t="s">
-        <v>8</v>
       </c>
       <c r="D268">
         <v>2</v>
@@ -7443,10 +7444,10 @@
         <v>44461</v>
       </c>
       <c r="B269" t="s">
+        <v>15</v>
+      </c>
+      <c r="C269" t="s">
         <v>7</v>
-      </c>
-      <c r="C269" t="s">
-        <v>15</v>
       </c>
       <c r="D269">
         <v>2</v>
@@ -7457,10 +7458,10 @@
         <v>44461</v>
       </c>
       <c r="B270" t="s">
+        <v>11</v>
+      </c>
+      <c r="C270" t="s">
         <v>10</v>
-      </c>
-      <c r="C270" t="s">
-        <v>11</v>
       </c>
       <c r="D270">
         <v>2</v>
@@ -7471,19 +7472,13 @@
         <v>44461</v>
       </c>
       <c r="B271" t="s">
+        <v>14</v>
+      </c>
+      <c r="C271" t="s">
         <v>12</v>
       </c>
-      <c r="C271" t="s">
-        <v>14</v>
-      </c>
       <c r="D271">
         <v>2</v>
-      </c>
-    </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="D272">
-        <f>SUM(D1:D271)</f>
-        <v>715</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.4">
@@ -7491,42 +7486,42 @@
         <v>41</v>
       </c>
       <c r="B273" t="s">
+        <v>6</v>
+      </c>
+      <c r="C273" t="s">
         <v>7</v>
-      </c>
-      <c r="C273" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B274" t="s">
+        <v>8</v>
+      </c>
+      <c r="C274" t="s">
         <v>9</v>
-      </c>
-      <c r="C274" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B275" t="s">
+        <v>10</v>
+      </c>
+      <c r="C275" t="s">
         <v>11</v>
-      </c>
-      <c r="C275" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B276" t="s">
+        <v>12</v>
+      </c>
+      <c r="C276" t="s">
         <v>13</v>
-      </c>
-      <c r="C276" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B277" t="s">
+        <v>14</v>
+      </c>
+      <c r="C277" t="s">
         <v>15</v>
-      </c>
-      <c r="C277" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>